<commit_message>
booking confirmed msg added
</commit_message>
<xml_diff>
--- a/Defects.xlsx
+++ b/Defects.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\karnj\Documents\GitHub\SoftwareProject\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AD276A86-2D0C-447F-9089-1FE1D17D9F67}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3535EBB1-A068-485B-A8F7-078BED2EBEC3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-98" yWindow="-98" windowWidth="19396" windowHeight="11596" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -477,7 +477,7 @@
   <dimension ref="A1:D16"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B6" sqref="B6"/>
+      <selection activeCell="A9" sqref="A9:XFD9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -580,15 +580,15 @@
         <v>15</v>
       </c>
     </row>
-    <row r="9" spans="1:4" ht="28.5" x14ac:dyDescent="0.45">
-      <c r="A9" t="s">
+    <row r="9" spans="1:4" s="1" customFormat="1" ht="28.5" x14ac:dyDescent="0.45">
+      <c r="A9" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="B9" s="2" t="s">
+      <c r="B9" s="3" t="s">
         <v>23</v>
       </c>
-      <c r="C9" t="s">
-        <v>5</v>
+      <c r="C9" s="1" t="s">
+        <v>15</v>
       </c>
     </row>
     <row r="10" spans="1:4" s="1" customFormat="1" ht="28.5" x14ac:dyDescent="0.45">

</xml_diff>

<commit_message>
Added one more defect
</commit_message>
<xml_diff>
--- a/Defects.xlsx
+++ b/Defects.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\karnj\Documents\GitHub\SoftwareProject\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://smuhalifax-my.sharepoint.com/personal/suchandra_ghosh_smu_ca/Documents/GitHub/SoftwareDevelopmentProject/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3535EBB1-A068-485B-A8F7-078BED2EBEC3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="4" documentId="13_ncr:1_{3535EBB1-A068-485B-A8F7-078BED2EBEC3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{AA28A4FE-276E-4D29-A351-1AB0965F6D2A}"/>
   <bookViews>
-    <workbookView xWindow="-98" yWindow="-98" windowWidth="19396" windowHeight="11596" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="41" uniqueCount="32">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="44" uniqueCount="35">
   <si>
     <t>Defect ID</t>
   </si>
@@ -121,6 +121,15 @@
   </si>
   <si>
     <t>D015</t>
+  </si>
+  <si>
+    <t>Rejected</t>
+  </si>
+  <si>
+    <t>Working as per requirement specified in assignment.</t>
+  </si>
+  <si>
+    <t>On clicking FAQ, exception is occuring.</t>
   </si>
 </sst>
 </file>
@@ -477,17 +486,17 @@
   <dimension ref="A1:D16"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A9" sqref="A9:XFD9"/>
+      <selection activeCell="D13" sqref="D13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="11.265625" customWidth="1"/>
-    <col min="2" max="2" width="68.86328125" style="2" customWidth="1"/>
-    <col min="4" max="4" width="57.86328125" customWidth="1"/>
+    <col min="1" max="1" width="11.28515625" customWidth="1"/>
+    <col min="2" max="2" width="68.85546875" style="2" customWidth="1"/>
+    <col min="4" max="4" width="57.85546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -501,7 +510,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="2" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.45">
+    <row r="2" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
         <v>3</v>
       </c>
@@ -512,7 +521,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="3" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.45">
+    <row r="3" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
         <v>6</v>
       </c>
@@ -523,7 +532,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
         <v>8</v>
       </c>
@@ -535,7 +544,7 @@
       </c>
       <c r="D4" s="1"/>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
         <v>10</v>
       </c>
@@ -547,7 +556,7 @@
       </c>
       <c r="D5" s="1"/>
     </row>
-    <row r="6" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.45">
+    <row r="6" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
         <v>12</v>
       </c>
@@ -558,7 +567,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="7" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.45">
+    <row r="7" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
         <v>16</v>
       </c>
@@ -569,7 +578,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="8" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.45">
+    <row r="8" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A8" s="1" t="s">
         <v>19</v>
       </c>
@@ -580,7 +589,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="9" spans="1:4" s="1" customFormat="1" ht="28.5" x14ac:dyDescent="0.45">
+    <row r="9" spans="1:4" s="1" customFormat="1" ht="30" x14ac:dyDescent="0.25">
       <c r="A9" s="1" t="s">
         <v>20</v>
       </c>
@@ -591,7 +600,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="10" spans="1:4" s="1" customFormat="1" ht="28.5" x14ac:dyDescent="0.45">
+    <row r="10" spans="1:4" s="1" customFormat="1" ht="30" x14ac:dyDescent="0.25">
       <c r="A10" s="1" t="s">
         <v>21</v>
       </c>
@@ -602,7 +611,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>22</v>
       </c>
@@ -610,10 +619,13 @@
         <v>25</v>
       </c>
       <c r="C11" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="12" spans="1:4" s="1" customFormat="1" ht="28.5" x14ac:dyDescent="0.45">
+        <v>32</v>
+      </c>
+      <c r="D11" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" s="1" customFormat="1" ht="45" x14ac:dyDescent="0.25">
       <c r="A12" s="1" t="s">
         <v>27</v>
       </c>
@@ -624,22 +636,28 @@
         <v>15</v>
       </c>
     </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>28</v>
       </c>
-    </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="B13" s="2" t="s">
+        <v>34</v>
+      </c>
+      <c r="C13" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>29</v>
       </c>
     </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>30</v>
       </c>
     </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>31</v>
       </c>

</xml_diff>

<commit_message>
Revert "Revert "Update azure-pipelines.yml""
This reverts commit a89e5db811b7059a115fdf1a0780943e4762fd2f, reversing
changes made to 1f6109372a71a136d28bedbcd97d80190f5d5b8c.
</commit_message>
<xml_diff>
--- a/Defects.xlsx
+++ b/Defects.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://smuhalifax-my.sharepoint.com/personal/suchandra_ghosh_smu_ca/Documents/GitHub/SoftwareDevelopmentProject/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\karnj\Documents\GitHub\SoftwareProject\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="4" documentId="13_ncr:1_{3535EBB1-A068-485B-A8F7-078BED2EBEC3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{AA28A4FE-276E-4D29-A351-1AB0965F6D2A}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3535EBB1-A068-485B-A8F7-078BED2EBEC3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-98" yWindow="-98" windowWidth="19396" windowHeight="11596" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="44" uniqueCount="35">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="41" uniqueCount="32">
   <si>
     <t>Defect ID</t>
   </si>
@@ -121,15 +121,6 @@
   </si>
   <si>
     <t>D015</t>
-  </si>
-  <si>
-    <t>Rejected</t>
-  </si>
-  <si>
-    <t>Working as per requirement specified in assignment.</t>
-  </si>
-  <si>
-    <t>On clicking FAQ, exception is occuring.</t>
   </si>
 </sst>
 </file>
@@ -486,17 +477,17 @@
   <dimension ref="A1:D16"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D13" sqref="D13"/>
+      <selection activeCell="A9" sqref="A9:XFD9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <cols>
-    <col min="1" max="1" width="11.28515625" customWidth="1"/>
-    <col min="2" max="2" width="68.85546875" style="2" customWidth="1"/>
-    <col min="4" max="4" width="57.85546875" customWidth="1"/>
+    <col min="1" max="1" width="11.265625" customWidth="1"/>
+    <col min="2" max="2" width="68.86328125" style="2" customWidth="1"/>
+    <col min="4" max="4" width="57.86328125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -510,7 +501,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="2" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.45">
       <c r="A2" s="1" t="s">
         <v>3</v>
       </c>
@@ -521,7 +512,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="3" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.45">
       <c r="A3" s="1" t="s">
         <v>6</v>
       </c>
@@ -532,7 +523,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A4" s="1" t="s">
         <v>8</v>
       </c>
@@ -544,7 +535,7 @@
       </c>
       <c r="D4" s="1"/>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A5" s="1" t="s">
         <v>10</v>
       </c>
@@ -556,7 +547,7 @@
       </c>
       <c r="D5" s="1"/>
     </row>
-    <row r="6" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.45">
       <c r="A6" s="1" t="s">
         <v>12</v>
       </c>
@@ -567,7 +558,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="7" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.45">
       <c r="A7" s="1" t="s">
         <v>16</v>
       </c>
@@ -578,7 +569,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="8" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.45">
       <c r="A8" s="1" t="s">
         <v>19</v>
       </c>
@@ -589,7 +580,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="9" spans="1:4" s="1" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:4" s="1" customFormat="1" ht="28.5" x14ac:dyDescent="0.45">
       <c r="A9" s="1" t="s">
         <v>20</v>
       </c>
@@ -600,7 +591,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="10" spans="1:4" s="1" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:4" s="1" customFormat="1" ht="28.5" x14ac:dyDescent="0.45">
       <c r="A10" s="1" t="s">
         <v>21</v>
       </c>
@@ -611,7 +602,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A11" t="s">
         <v>22</v>
       </c>
@@ -619,13 +610,10 @@
         <v>25</v>
       </c>
       <c r="C11" t="s">
-        <v>32</v>
-      </c>
-      <c r="D11" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="12" spans="1:4" s="1" customFormat="1" ht="45" x14ac:dyDescent="0.25">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" s="1" customFormat="1" ht="28.5" x14ac:dyDescent="0.45">
       <c r="A12" s="1" t="s">
         <v>27</v>
       </c>
@@ -636,28 +624,22 @@
         <v>15</v>
       </c>
     </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A13" t="s">
         <v>28</v>
       </c>
-      <c r="B13" s="2" t="s">
-        <v>34</v>
-      </c>
-      <c r="C13" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
+    </row>
+    <row r="14" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A14" t="s">
         <v>29</v>
       </c>
     </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A15" t="s">
         <v>30</v>
       </c>
     </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A16" t="s">
         <v>31</v>
       </c>

</xml_diff>